<commit_message>
Checkpoint 8. Integration with GUI: arduino now will try to parse string array received from the Serial Interface into 4 chunks of NFC memory bytes and writes every value of the chunk back on the serial interface. NFC memory writing to be implemented
</commit_message>
<xml_diff>
--- a/register_values.xlsx
+++ b/register_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edvar\Google Drive\Study\2021\UCL 2 year\MRes Project\User manual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/rmaperu_ucl_ac_uk/Documents/MRes sVNS project/MRes Project/Firmwares/PN532_custom/readMifare/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32393EF8-352C-4AE4-B63F-1F794B8B009A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -646,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -681,16 +679,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -733,6 +727,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -744,30 +741,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -861,6 +834,30 @@
     </dxf>
     <dxf>
       <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -876,12 +873,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F05B536-2AC8-4C21-9473-95D013DC001F}" name="Table1" displayName="Table1" ref="G7:I15" totalsRowShown="0" headerRowDxfId="0" dataDxfId="7" headerRowBorderDxfId="1" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F05B536-2AC8-4C21-9473-95D013DC001F}" name="Table1" displayName="Table1" ref="G7:I15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="G7:I15" xr:uid="{6F05B536-2AC8-4C21-9473-95D013DC001F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{ABE48319-BD0D-497A-993C-DA1553FA2E62}" name="Reload byte word" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{450DDC52-BCF2-4290-B21F-3F7296BD2085}" name="Seconds" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{721BE083-DE33-4DA2-850B-CEC9F7160A7A}" name="Data array values" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{ABE48319-BD0D-497A-993C-DA1553FA2E62}" name="Reload byte word" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{450DDC52-BCF2-4290-B21F-3F7296BD2085}" name="Seconds" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{721BE083-DE33-4DA2-850B-CEC9F7160A7A}" name="Data array values" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1152,26 +1149,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.81640625" customWidth="1"/>
+    <col min="5" max="5" width="22.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" customWidth="1"/>
+    <col min="9" max="9" width="16.26953125" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -1186,7 +1183,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1199,7 +1196,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -1216,7 +1213,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
@@ -1229,11 +1226,11 @@
       <c r="D4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
@@ -1246,30 +1243,29 @@
       <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="G5" s="13" t="s">
+      <c r="E5" s="32"/>
+      <c r="G5" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
-      <c r="K5" s="34" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
+      <c r="K5" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="L5" s="35"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="34"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="10"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="18"/>
-    </row>
-    <row r="7" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="15"/>
+      <c r="I6" s="16"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
+    </row>
+    <row r="7" spans="1:12" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -1282,26 +1278,26 @@
       <c r="D7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="16">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
@@ -1314,25 +1310,25 @@
       <c r="D8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="G8" s="27" t="s">
+      <c r="E8" s="32"/>
+      <c r="G8" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="26">
         <v>1</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="L8" s="33">
+      <c r="L8" s="31">
         <f>L7/(2012/64)</f>
         <v>4.071570576540755</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
@@ -1345,18 +1341,18 @@
       <c r="D9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="G9" s="22" t="s">
+      <c r="E9" s="32"/>
+      <c r="G9" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="18">
         <v>5</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
@@ -1372,33 +1368,33 @@
       <c r="E10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="18">
         <v>10</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="18">
         <v>20</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>23</v>
       </c>
@@ -1414,17 +1410,17 @@
       <c r="E12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="18">
         <v>30</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
@@ -1438,17 +1434,17 @@
         <v>57</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="18">
         <v>50</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="21" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>25</v>
       </c>
@@ -1464,17 +1460,17 @@
       <c r="E14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="18">
         <v>60</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
@@ -1482,24 +1478,24 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="23">
         <v>120</v>
       </c>
-      <c r="I15" s="26" t="s">
+      <c r="I15" s="24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="10"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>30</v>
       </c>
@@ -1514,7 +1510,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>31</v>
       </c>
@@ -1523,7 +1519,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>32</v>
       </c>
@@ -1532,7 +1528,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="11" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Checkpoint 13a. Decreased NT3H interrogation time to 200 ms (5 Hz) to make triggering more stable.
</commit_message>
<xml_diff>
--- a/register_values.xlsx
+++ b/register_values.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/rmaperu_ucl_ac_uk/Documents/MRes sVNS project/MRes Project/Firmwares/PN532_custom/readMifare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32393EF8-352C-4AE4-B63F-1F794B8B009A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="13_ncr:1_{32393EF8-352C-4AE4-B63F-1F794B8B009A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35FAF4FB-90DF-49F1-AD18-1CC0BC4FA620}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="Programming_revised" sheetId="3" r:id="rId1"/>
+    <sheet name="18.07.2023 Programming" sheetId="2" r:id="rId2"/>
+    <sheet name="List1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="159">
   <si>
     <t>Parameter</t>
   </si>
@@ -283,13 +285,317 @@
   </si>
   <si>
     <t>Page 6, Byte 0:</t>
+  </si>
+  <si>
+    <t>Programming data stored in 3 NFC SRAM pages: 4, 5, 6</t>
+  </si>
+  <si>
+    <t>Example pages (in HEX):</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00:01:03:E6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - PW high byte, PW low byte, Period high byte, Period low byte
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00:01:00:01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Stimulation On high byte, Stimulation On low byte, 0, On/Off
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3F:03:00:01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Current, Mode, Channel Number, Telemetry On/Off</t>
+    </r>
+  </si>
+  <si>
+    <t>Pulse width (high byte, low byte): number x 50 us</t>
+  </si>
+  <si>
+    <t>1 to 80</t>
+  </si>
+  <si>
+    <t>pulse width, s</t>
+  </si>
+  <si>
+    <t>period, s</t>
+  </si>
+  <si>
+    <t>Programming values:</t>
+  </si>
+  <si>
+    <t>Programming values (HEX):</t>
+  </si>
+  <si>
+    <t>Pulse width and period calculations:</t>
+  </si>
+  <si>
+    <t>HEX to DEC calculator:</t>
+  </si>
+  <si>
+    <t>Stimulation On/Off:</t>
+  </si>
+  <si>
+    <t>time in seconds</t>
+  </si>
+  <si>
+    <t>On/Off</t>
+  </si>
+  <si>
+    <t>1/0</t>
+  </si>
+  <si>
+    <t>Current: see table</t>
+  </si>
+  <si>
+    <t>Table of current levels:</t>
+  </si>
+  <si>
+    <t>dec set</t>
+  </si>
+  <si>
+    <t>hex set</t>
+  </si>
+  <si>
+    <t>IREF set, mA</t>
+  </si>
+  <si>
+    <t>device current set, mA, no coefficient</t>
+  </si>
+  <si>
+    <t>device current set, mA</t>
+  </si>
+  <si>
+    <t>3F</t>
+  </si>
+  <si>
+    <t>3E</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>2F</t>
+  </si>
+  <si>
+    <t>2E</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>1F</t>
+  </si>
+  <si>
+    <t>1E</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>0F</t>
+  </si>
+  <si>
+    <t>0E</t>
+  </si>
+  <si>
+    <t>0D</t>
+  </si>
+  <si>
+    <t>0C</t>
+  </si>
+  <si>
+    <t>0B</t>
+  </si>
+  <si>
+    <t>0A</t>
+  </si>
+  <si>
+    <t>Channel number:</t>
+  </si>
+  <si>
+    <t>0 to 14</t>
+  </si>
+  <si>
+    <t>Mode:</t>
+  </si>
+  <si>
+    <t>2 for single scan and then stop after last channel stimulated</t>
+  </si>
+  <si>
+    <t>3 for scanning loop</t>
+  </si>
+  <si>
+    <t>1 for single channel stim (specify channel)</t>
+  </si>
+  <si>
+    <t>Telemetry on/off:</t>
+  </si>
+  <si>
+    <t>0 for disabling channel writing to NFC</t>
+  </si>
+  <si>
+    <t>1 to enable current stimulation channel to NFC</t>
+  </si>
+  <si>
+    <t>DEC to HEX calculator</t>
+  </si>
+  <si>
+    <t>&lt;0,2,3,228,0,2,0,1,63,3,0,1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Combine all data in a single string:</t>
+  </si>
+  <si>
+    <t>100 uA</t>
+  </si>
+  <si>
+    <t>150 uA</t>
+  </si>
+  <si>
+    <t>200 uA</t>
+  </si>
+  <si>
+    <t>300 uA</t>
+  </si>
+  <si>
+    <t>50 us</t>
+  </si>
+  <si>
+    <t>1 ms</t>
+  </si>
+  <si>
+    <t>2 ms</t>
+  </si>
+  <si>
+    <t>10 Hz</t>
+  </si>
+  <si>
+    <t>20 Hz</t>
+  </si>
+  <si>
+    <t>1 mA</t>
+  </si>
+  <si>
+    <t>2 mA</t>
+  </si>
+  <si>
+    <t>10Hz</t>
+  </si>
+  <si>
+    <t>PW         T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Ton</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">          I     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mode</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;00,01,03,230,00,5,00,01,63,03,00,01&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,13 +617,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="27">
@@ -644,7 +963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -727,6 +1046,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1146,10 +1474,1660 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2813CE-5935-4F3E-858D-87B79A4CA860}">
+  <dimension ref="B2:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" s="1">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="36"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="1">
+        <v>20</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="36"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="1">
+        <v>40</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="1">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="1">
+        <v>30</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE542E2-DB77-474C-AC1D-5EC2409B853E}">
+  <dimension ref="B2:O68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="49.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="87" x14ac:dyDescent="0.35">
+      <c r="B4" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="N4" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" s="33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="K5">
+        <v>63</v>
+      </c>
+      <c r="L5" t="s">
+        <v>105</v>
+      </c>
+      <c r="M5">
+        <f>K5*0.008</f>
+        <v>0.504</v>
+      </c>
+      <c r="N5">
+        <f>M5*4</f>
+        <v>2.016</v>
+      </c>
+      <c r="O5">
+        <f>N5+0.05*N5</f>
+        <v>2.1168</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6">
+        <v>62</v>
+      </c>
+      <c r="L6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M68" si="0">K6*0.008</f>
+        <v>0.496</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N68" si="1">M6*4</f>
+        <v>1.984</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O68" si="2">N6+0.05*N6</f>
+        <v>2.0832000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7">
+        <v>61</v>
+      </c>
+      <c r="L7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>1.952</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>2.0495999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8">
+        <v>60</v>
+      </c>
+      <c r="L8" t="s">
+        <v>108</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>1.92</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>2.016</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C9" s="34">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="D9" s="35">
+        <f>1/20</f>
+        <v>0.05</v>
+      </c>
+      <c r="I9" t="s">
+        <v>140</v>
+      </c>
+      <c r="K9">
+        <v>59</v>
+      </c>
+      <c r="L9" t="s">
+        <v>109</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>0.47200000000000003</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>1.8880000000000001</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>1.9824000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <f>0.00005</f>
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>58</v>
+      </c>
+      <c r="L10" t="s">
+        <v>110</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>1.8560000000000001</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>1.9488000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <f>D9/D10</f>
+        <v>1000</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>57</v>
+      </c>
+      <c r="L11">
+        <v>39</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>1.8240000000000001</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>1.9152</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <v>56</v>
+      </c>
+      <c r="L12">
+        <v>38</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>1.792</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>1.8816000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13">
+        <f>C9/0.00005</f>
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f>D11-2*C13</f>
+        <v>998</v>
+      </c>
+      <c r="I13">
+        <v>228</v>
+      </c>
+      <c r="K13">
+        <v>55</v>
+      </c>
+      <c r="L13">
+        <v>37</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0.44</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>1.76</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>1.8480000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="str">
+        <f>DEC2HEX(D13)</f>
+        <v>3E6</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>54</v>
+      </c>
+      <c r="L14">
+        <v>36</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>0.432</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>1.728</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="2"/>
+        <v>1.8144</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15">
+        <v>98</v>
+      </c>
+      <c r="D15">
+        <f>HEX2DEC(C15)</f>
+        <v>152</v>
+      </c>
+      <c r="K15">
+        <v>53</v>
+      </c>
+      <c r="L15">
+        <v>35</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>1.696</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>1.7807999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <v>52</v>
+      </c>
+      <c r="L16">
+        <v>34</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>0.41600000000000004</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>1.6640000000000001</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="2"/>
+        <v>1.7472000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" t="s">
+        <v>95</v>
+      </c>
+      <c r="K17">
+        <v>51</v>
+      </c>
+      <c r="L17">
+        <v>33</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>0.40800000000000003</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>1.6320000000000001</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="2"/>
+        <v>1.7136</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18" t="str">
+        <f>DEC2HEX(C18)</f>
+        <v>14</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>50</v>
+      </c>
+      <c r="L18">
+        <v>32</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="2"/>
+        <v>1.6800000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>49</v>
+      </c>
+      <c r="L19">
+        <v>31</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="2"/>
+        <v>1.6464000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>48</v>
+      </c>
+      <c r="L20">
+        <v>30</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>1.536</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>1.6128</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21">
+        <v>63</v>
+      </c>
+      <c r="K21">
+        <v>47</v>
+      </c>
+      <c r="L21" t="s">
+        <v>111</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>0.376</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>1.504</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>1.5791999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="K22">
+        <v>46</v>
+      </c>
+      <c r="L22" t="s">
+        <v>112</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>1.472</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="2"/>
+        <v>1.5455999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" t="s">
+        <v>134</v>
+      </c>
+      <c r="K23">
+        <v>45</v>
+      </c>
+      <c r="L23" t="s">
+        <v>113</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>1.44</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="2"/>
+        <v>1.512</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>132</v>
+      </c>
+      <c r="K24">
+        <v>44</v>
+      </c>
+      <c r="L24" t="s">
+        <v>114</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="2"/>
+        <v>1.4783999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>133</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <v>43</v>
+      </c>
+      <c r="L25" t="s">
+        <v>115</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>0.34400000000000003</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>1.3760000000000001</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="2"/>
+        <v>1.4448000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="K26">
+        <v>42</v>
+      </c>
+      <c r="L26" t="s">
+        <v>116</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>1.3440000000000001</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="2"/>
+        <v>1.4112</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" t="s">
+        <v>130</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>41</v>
+      </c>
+      <c r="L27">
+        <v>29</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>1.3120000000000001</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="2"/>
+        <v>1.3776000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="K28">
+        <v>40</v>
+      </c>
+      <c r="L28">
+        <v>28</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>1.28</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="2"/>
+        <v>1.3440000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" t="s">
+        <v>136</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>39</v>
+      </c>
+      <c r="L29">
+        <v>27</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>0.312</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>1.248</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="2"/>
+        <v>1.3104</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>137</v>
+      </c>
+      <c r="I30" t="s">
+        <v>141</v>
+      </c>
+      <c r="K30">
+        <v>38</v>
+      </c>
+      <c r="L30">
+        <v>26</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>1.216</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="2"/>
+        <v>1.2767999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="K31">
+        <v>37</v>
+      </c>
+      <c r="L31">
+        <v>25</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>1.1839999999999999</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="2"/>
+        <v>1.2431999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="K32">
+        <v>36</v>
+      </c>
+      <c r="L32">
+        <v>24</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>0.28800000000000003</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>1.1520000000000001</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="2"/>
+        <v>1.2096000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K33">
+        <v>35</v>
+      </c>
+      <c r="L33">
+        <v>23</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="2"/>
+        <v>1.1760000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K34">
+        <v>34</v>
+      </c>
+      <c r="L34">
+        <v>22</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="0"/>
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>1.0880000000000001</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="2"/>
+        <v>1.1424000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K35">
+        <v>33</v>
+      </c>
+      <c r="L35">
+        <v>21</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>1.056</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="2"/>
+        <v>1.1088</v>
+      </c>
+    </row>
+    <row r="36" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K36">
+        <v>32</v>
+      </c>
+      <c r="L36">
+        <v>20</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="0"/>
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="1"/>
+        <v>1.024</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="2"/>
+        <v>1.0751999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K37">
+        <v>31</v>
+      </c>
+      <c r="L37" t="s">
+        <v>117</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="0"/>
+        <v>0.248</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="1"/>
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="2"/>
+        <v>1.0416000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K38">
+        <v>30</v>
+      </c>
+      <c r="L38" t="s">
+        <v>118</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="1"/>
+        <v>0.96</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="2"/>
+        <v>1.008</v>
+      </c>
+    </row>
+    <row r="39" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K39">
+        <v>29</v>
+      </c>
+      <c r="L39" t="s">
+        <v>119</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="0"/>
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="1"/>
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="2"/>
+        <v>0.97440000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K40">
+        <v>28</v>
+      </c>
+      <c r="L40" t="s">
+        <v>120</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="0"/>
+        <v>0.224</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="1"/>
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="2"/>
+        <v>0.94080000000000008</v>
+      </c>
+    </row>
+    <row r="41" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K41">
+        <v>27</v>
+      </c>
+      <c r="L41" t="s">
+        <v>121</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="0"/>
+        <v>0.216</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="1"/>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="2"/>
+        <v>0.90720000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K42">
+        <v>26</v>
+      </c>
+      <c r="L42" t="s">
+        <v>122</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="0"/>
+        <v>0.20800000000000002</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="1"/>
+        <v>0.83200000000000007</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="2"/>
+        <v>0.87360000000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K43">
+        <v>25</v>
+      </c>
+      <c r="L43">
+        <v>19</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="2"/>
+        <v>0.84000000000000008</v>
+      </c>
+    </row>
+    <row r="44" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K44">
+        <v>24</v>
+      </c>
+      <c r="L44">
+        <v>18</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="0"/>
+        <v>0.192</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="1"/>
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="2"/>
+        <v>0.80640000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K45">
+        <v>23</v>
+      </c>
+      <c r="L45">
+        <v>17</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="0"/>
+        <v>0.184</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="1"/>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="2"/>
+        <v>0.77279999999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K46">
+        <v>22</v>
+      </c>
+      <c r="L46">
+        <v>16</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="0"/>
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="1"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="2"/>
+        <v>0.73919999999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K47">
+        <v>21</v>
+      </c>
+      <c r="L47">
+        <v>15</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="0"/>
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="1"/>
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="2"/>
+        <v>0.7056</v>
+      </c>
+    </row>
+    <row r="48" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K48">
+        <v>20</v>
+      </c>
+      <c r="L48">
+        <v>14</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="1"/>
+        <v>0.64</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="2"/>
+        <v>0.67200000000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K49">
+        <v>19</v>
+      </c>
+      <c r="L49">
+        <v>13</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="0"/>
+        <v>0.152</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="1"/>
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="2"/>
+        <v>0.63839999999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K50">
+        <v>18</v>
+      </c>
+      <c r="L50">
+        <v>12</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="0"/>
+        <v>0.14400000000000002</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="1"/>
+        <v>0.57600000000000007</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="2"/>
+        <v>0.60480000000000012</v>
+      </c>
+    </row>
+    <row r="51" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K51">
+        <v>17</v>
+      </c>
+      <c r="L51">
+        <v>11</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="0"/>
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="1"/>
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="2"/>
+        <v>0.57120000000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K52">
+        <v>16</v>
+      </c>
+      <c r="L52">
+        <v>10</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="0"/>
+        <v>0.128</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="1"/>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="2"/>
+        <v>0.53759999999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K53">
+        <v>15</v>
+      </c>
+      <c r="L53" t="s">
+        <v>123</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="2"/>
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="54" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K54">
+        <v>14</v>
+      </c>
+      <c r="L54" t="s">
+        <v>124</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="0"/>
+        <v>0.112</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="1"/>
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="2"/>
+        <v>0.47040000000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K55">
+        <v>13</v>
+      </c>
+      <c r="L55" t="s">
+        <v>125</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="0"/>
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="1"/>
+        <v>0.41600000000000004</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="2"/>
+        <v>0.43680000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K56">
+        <v>12</v>
+      </c>
+      <c r="L56" t="s">
+        <v>126</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="1"/>
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="2"/>
+        <v>0.4032</v>
+      </c>
+    </row>
+    <row r="57" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K57">
+        <v>11</v>
+      </c>
+      <c r="L57" t="s">
+        <v>127</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="0"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="1"/>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="2"/>
+        <v>0.36959999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K58">
+        <v>10</v>
+      </c>
+      <c r="L58" t="s">
+        <v>128</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="1"/>
+        <v>0.32</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="2"/>
+        <v>0.33600000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K59">
+        <v>9</v>
+      </c>
+      <c r="L59">
+        <v>9</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000008E-2</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="1"/>
+        <v>0.28800000000000003</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="2"/>
+        <v>0.30240000000000006</v>
+      </c>
+    </row>
+    <row r="60" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K60">
+        <v>8</v>
+      </c>
+      <c r="L60">
+        <v>8</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="0"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="1"/>
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="2"/>
+        <v>0.26879999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K61">
+        <v>7</v>
+      </c>
+      <c r="L61">
+        <v>7</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="0"/>
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="1"/>
+        <v>0.224</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="2"/>
+        <v>0.23520000000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K62">
+        <v>6</v>
+      </c>
+      <c r="L62">
+        <v>6</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="1"/>
+        <v>0.192</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="2"/>
+        <v>0.2016</v>
+      </c>
+    </row>
+    <row r="63" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K63">
+        <v>5</v>
+      </c>
+      <c r="L63">
+        <v>5</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="1"/>
+        <v>0.16</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="2"/>
+        <v>0.16800000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K64">
+        <v>4</v>
+      </c>
+      <c r="L64">
+        <v>4</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="0"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="1"/>
+        <v>0.128</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="2"/>
+        <v>0.13439999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K65">
+        <v>3</v>
+      </c>
+      <c r="L65">
+        <v>3</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="1"/>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="2"/>
+        <v>0.1008</v>
+      </c>
+    </row>
+    <row r="66" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K66">
+        <v>2</v>
+      </c>
+      <c r="L66">
+        <v>2</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="0"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="1"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="2"/>
+        <v>6.7199999999999996E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="2"/>
+        <v>3.3599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1226,7 +3204,7 @@
       <c r="D4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="37" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1243,16 +3221,16 @@
       <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="37"/>
       <c r="G5" s="12" t="s">
         <v>79</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="14"/>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="L5" s="34"/>
+      <c r="L5" s="39"/>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="10"/>
@@ -1278,7 +3256,7 @@
       <c r="D7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="37" t="s">
         <v>53</v>
       </c>
       <c r="G7" s="28" t="s">
@@ -1310,7 +3288,7 @@
       <c r="D8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="37"/>
       <c r="G8" s="25" t="s">
         <v>61</v>
       </c>
@@ -1341,7 +3319,7 @@
       <c r="D9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="37"/>
       <c r="G9" s="20" t="s">
         <v>62</v>
       </c>

</xml_diff>